<commit_message>
Change of Excel Template for SAS
</commit_message>
<xml_diff>
--- a/source-code/mmria/mmria-server/database-scripts/Template.xlsx
+++ b/source-code/mmria/mmria-server/database-scripts/Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\source\repos\FastExcel-Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cdc-my.sharepoint.com/personal/qha1_cdc_gov/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFA0781B-C969-445B-BAFD-9EFB50E09405}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{01EF27BC-8825-4D92-BC4A-7538041E6CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12045" yWindow="0" windowWidth="16755" windowHeight="15600" xr2:uid="{9F6A6042-26C5-4446-A0CE-786D65AD59A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{89FF205D-4F73-495D-A169-B4F8B4A889B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -379,7 +379,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C685993-2301-40F2-9702-3294D1BBFEAA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F76AC18-B1EC-48F0-94CE-4E7FD069E72D}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -387,5 +387,6 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>